<commit_message>
Working on ferredoxin fixing
</commit_message>
<xml_diff>
--- a/Matt_Work/double_dead_ends.xlsx
+++ b/Matt_Work/double_dead_ends.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="132" windowWidth="14340" windowHeight="5832"/>
+    <workbookView xWindow="384" yWindow="84" windowWidth="14340" windowHeight="7944"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,332 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+  <si>
+    <t>rxn01025_c0</t>
+  </si>
+  <si>
+    <t>5-Methylcytosine aminohydrolase c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H_c0 + H2O_c0 + 5-Methylcytosine_c0  -&gt; NH3_c0 + Thymine_c0 </t>
+  </si>
+  <si>
+    <t>rxn01241_c0</t>
+  </si>
+  <si>
+    <t>Dihydrolipoamide NAD oxidoreductase c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAD_c0 + Dihydrolipoamide_c0  &lt;=&gt; H_c0 + NADH_c0 + Lipoamide_c0 </t>
+  </si>
+  <si>
+    <t>rxn01329_c0</t>
+  </si>
+  <si>
+    <t>D-Mannose 6-phosphate 1 6-phosphomutase c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-mannose-6-phosphate_c0  &lt;=&gt; D-Mannose1-phosphate_c0 </t>
+  </si>
+  <si>
+    <t>rxn01620_c0</t>
+  </si>
+  <si>
+    <t>L-Fuculose-1-phosphate lactaldehyde-lyase c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Fuculose1-phosphate_c0  &lt;=&gt; Glycerone-phosphate_c0 + L-Lactaldehyde_c0 </t>
+  </si>
+  <si>
+    <t>rxn01664_c0</t>
+  </si>
+  <si>
+    <t>2-Aminoadipate 6-semialdehyde c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Aminoadipate_6-semialdehyde_c0  -&gt; H_c0 + H2O_c0 + delta1-Piperideine-6-L-carboxylate_c0 </t>
+  </si>
+  <si>
+    <t>rxn02339_c0</t>
+  </si>
+  <si>
+    <t>4-Hydroxy-L-glutamate 2-oxoglutarate aminotransferase c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Oxoglutarate_c0 + 4-Hydroxy-L-glutamate_c0  &lt;=&gt; L-Glutamate_c0 + 4-Hydroxy-2-oxoglutarate_c0 </t>
+  </si>
+  <si>
+    <t>rxn02374_c0</t>
+  </si>
+  <si>
+    <t>L-glutamate 5-semialdehyde dehydratase spontaneous c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Glutamate5-semialdehyde_c0  -&gt; H_c0 + H2O_c0 + 1-Pyrroline-5-carboxylate_c0 </t>
+  </si>
+  <si>
+    <t>rxn02483_c0</t>
+  </si>
+  <si>
+    <t>4-Carboxymuconolactone carboxy-lyase c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H_c0 + 4-Carboxymuconolactone_c0  -&gt; 3-oxoadipate-enol-lactone_c0 + CO2_c0 </t>
+  </si>
+  <si>
+    <t>rxn02569_c0</t>
+  </si>
+  <si>
+    <t>ATP selenide water phosphotransferase c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2O_c0 + ATP_c0 + Selenide_c0  &lt;=&gt; 2 H_c0 + Phosphate_c0 + AMP_c0 + Selenophosphate_c0 </t>
+  </si>
+  <si>
+    <t>rxn02916_c0</t>
+  </si>
+  <si>
+    <t>6-Amino-2-oxohexanoate cyclation c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Oxo-6-aminocaproate_c0  -&gt; H_c0 + H2O_c0 + delta1-Piperideine-2-carboxylate_c0 </t>
+  </si>
+  <si>
+    <t>rxn03126_c0</t>
+  </si>
+  <si>
+    <t>Coenzyme B coenzyme M methanophenazine oxidoreductase c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CoM-S-S-CoB_c0 + Dihydromethanophenazine_c0  -&gt; CoM_c0 + Methanophenazine_c0 + HTP_c0 </t>
+  </si>
+  <si>
+    <t>rxn03406_c0</t>
+  </si>
+  <si>
+    <t>Undecaprenyl-diphospho-N-acetylmuramoyl-N-acetylglucosamine- c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATP_c0 + NH3_c0 + Undecaprenyl-diphospho-N-acetylmuramoyl-N-acetylglucosamine-L-alanyl-D-glutamyl-L-lysyl-D-alanyl-D-alanine_c0  -&gt; H_c0 + Phosphate_c0 + ADP_c0 + Undecaprenyl-diphospho-N-acetylmuramoyl-N-acetylglucosamine-L-alanyl-D-glutaminyl-L-lysyl-D-alanyl-D-alanine_c0 </t>
+  </si>
+  <si>
+    <t>rxn03407_c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATP_c0 + NH3_c0 + Undecaprenyl-diphospho-N-acetylmuramoyl-N-acetylglucosamine-L-alanyl-gamma-D-glutamyl-L-lysyl-D-alanyl-D-alanine_c0  -&gt; H_c0 + Phosphate_c0 + ADP_c0 + Undecaprenyl-diphospho-N-acetylmuramoyl-N-acetylglucosamine-L-alanyl-D-isoglutaminyl-L-lysyl-D-alanyl-D-alanine_c0 </t>
+  </si>
+  <si>
+    <t>rxn03446_c0</t>
+  </si>
+  <si>
+    <t>O-Phospho-4-hydroxy-L-threonine phospho-lyase adding water c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2O_c0 + 4-Phosphonooxy-threonine_c0  -&gt; H_c0 + Phosphate_c0 + 4-Hydroxy-L-threonine_c0 </t>
+  </si>
+  <si>
+    <t>rxn04385_c0</t>
+  </si>
+  <si>
+    <t>L-threonine-O-3-phosphate carboxy-lyase c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H_c0 + L-Threonine_phosphate_c0  -&gt; CO2_c0 + R-1-Aminopropan-2-yl_phosphate_c0 </t>
+  </si>
+  <si>
+    <t>rxn05116_c0</t>
+  </si>
+  <si>
+    <t>rxn05116 c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H_c0 + 2-Amino-3-oxo-4-phosphonooxybutyrate_c0  -&gt; CO2_c0 + 3-Amino-2-oxopropyl_phosphate_c0 </t>
+  </si>
+  <si>
+    <t>rxn05171_c0</t>
+  </si>
+  <si>
+    <t>Nitrate-ABC transport c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2O_c0 + ATP_c0 + Nitrate_e0  -&gt; H_c0 + Phosphate_c0 + ADP_c0 + Nitrate_c0 </t>
+  </si>
+  <si>
+    <t>rxn05181_c0</t>
+  </si>
+  <si>
+    <t>Betaine-ABC transport c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2O_c0 + ATP_c0 + BET_e0  -&gt; H_c0 + Phosphate_c0 + ADP_c0 + BET_c0 </t>
+  </si>
+  <si>
+    <t>rxn05247_c0</t>
+  </si>
+  <si>
+    <t>FACOAL140ISO c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H_c0 + CoA_c0 + ATP_c0 + fa1_c0  -&gt; PPi_c0 + AMP_c0 + fa1coa_c0 </t>
+  </si>
+  <si>
+    <t>rxn05248_c0</t>
+  </si>
+  <si>
+    <t>FACOAL150anteiso c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H_c0 + CoA_c0 + ATP_c0 + fa4_c0  -&gt; PPi_c0 + AMP_c0 + fa4coa_c0 </t>
+  </si>
+  <si>
+    <t>rxn05249_c0</t>
+  </si>
+  <si>
+    <t>FACOAL150ISO c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H_c0 + CoA_c0 + ATP_c0 + fa3_c0  -&gt; PPi_c0 + AMP_c0 + fa3coa_c0 </t>
+  </si>
+  <si>
+    <t>rxn05250_c0</t>
+  </si>
+  <si>
+    <t>FACOAL160ISO c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H_c0 + CoA_c0 + ATP_c0 + fa6_c0  -&gt; PPi_c0 + AMP_c0 + fa6coa_c0 </t>
+  </si>
+  <si>
+    <t>rxn05740_c0</t>
+  </si>
+  <si>
+    <t>cpd00155 phosphorylase c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H_c0 + Phosphate_c0 + Glycogen_c0  &lt;=&gt; Glucose-1-phosphate_c0 + glycogenn-1_c0 </t>
+  </si>
+  <si>
+    <t>rxn06493_c0</t>
+  </si>
+  <si>
+    <t>dihydrolipoylprotein NAD oxidoreductase c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAD_c0 + Dihydrolipolprotein_c0  &lt;=&gt; H_c0 + NADH_c0 + Lipoylprotein_c0 </t>
+  </si>
+  <si>
+    <t>rxn08180_c0</t>
+  </si>
+  <si>
+    <t>Biotin synthase c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S-Adenosyl-L-methionine_c0 + Dethiobiotin_c0 + S_c0  -&gt; H_c0 + L-Methionine_c0 + 5'-Deoxyadenosine_c0 + BIOT_c0 </t>
+  </si>
+  <si>
+    <t>rxn09450_c0</t>
+  </si>
+  <si>
+    <t>fatty-acid--CoA ligase hexadecenoate peroxisomal c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H_c0 + CoA_c0 + ATP_c0 + hexadecenoate_c0  -&gt; PPi_c0 + AMP_c0 + Hexadecenoyl-CoA_c0 </t>
+  </si>
+  <si>
+    <t>rxn10307_c0</t>
+  </si>
+  <si>
+    <t>palmitoyl-lipoteichoic acid synthesis n=24 linked N-acetylglucosamine substituted c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 UDP-N-acetylglucosamine_c0 + Palmitoyllipoteichoic_acid_n=24__linked__unsubstituted_c0  &lt;=&gt; 24 UDP_c0 + Palmitoyllipoteichoic_acid_n=24__linked__N-acetyl-D-glucosamine_c0 </t>
+  </si>
+  <si>
+    <t>rxn10308_c0</t>
+  </si>
+  <si>
+    <t>myristoyl-lipoteichoic acid synthesis n=24 linked N-acetylglucosamine substituted c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myristoyllipoteichoic_acid_n=24__linked__unsubstituted_c0 + 24 UDP-N-acetylglucosamine_c0  &lt;=&gt; 24 UDP_c0 + Myristoyllipoteichoic_acid_n=24__linked__N-acetyl-D-glucosamine_c0 </t>
+  </si>
+  <si>
+    <t>rxn10309_c0</t>
+  </si>
+  <si>
+    <t>stearoyl-lipoteichoic acid synthesis n=24 linked N-acetylglucosamine substituted c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 UDP-N-acetylglucosamine_c0 + Stearoyllipoteichoic_acid_n=24__linked__unsubstituted_c0  &lt;=&gt; 24 UDP_c0 + Stearoyllipoteichoic_acid_n=24__linked__N-acetyl-D-glucosamine_c0 </t>
+  </si>
+  <si>
+    <t>rxn10310_c0</t>
+  </si>
+  <si>
+    <t>isoheptadecanoyl-lipoteichoic acid synthesis n=24 linked N-acetylglucosamine substituted c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 UDP-N-acetylglucosamine_c0 + Isoheptadecanoyllipoteichoic_acid_n=24__linked__unsubstituted_c0  &lt;=&gt; 24 UDP_c0 + Isoheptadecanoyllipoteichoic_acid_n=24__linked__N-acetyl-D-glucosamine_c0 </t>
+  </si>
+  <si>
+    <t>rxn10311_c0</t>
+  </si>
+  <si>
+    <t>anteisoheptadecanoyl-lipoteichoic acid synthesis n=24 linked N-acetylglucosamine substituted c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 UDP-N-acetylglucosamine_c0 + Anteisoheptadecanoyllipoteichoic_acid_n=24__linked__unsubstituted_c0  &lt;=&gt; 24 UDP_c0 + Anteisoheptadecanoyllipoteichoic_acid_n=24__linked__N-acetyl-D-glucosamine_c0 </t>
+  </si>
+  <si>
+    <t>rxn10312_c0</t>
+  </si>
+  <si>
+    <t>isotetradecanoyl-lipoteichoic acid synthesis n=24 linked N-acetylglucosamine substituted c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 UDP-N-acetylglucosamine_c0 + Isotetradecanoyllipoteichoic_acid_n=24__linked__unsubstituted_c0  &lt;=&gt; 24 UDP_c0 + Isotetradecanoyllipoteichoic_acid_n=24__linked__N-acetyl-D-glucosamine_c0 </t>
+  </si>
+  <si>
+    <t>rxn10313_c0</t>
+  </si>
+  <si>
+    <t>isopentadecanoyl-lipoteichoic acid synthesis n=24 linked N-acetylglucosamine substituted c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 UDP-N-acetylglucosamine_c0 + Isopentadecanoyllipoteichoic_acid_n=24__linked__unsubstituted_c0  &lt;=&gt; 24 UDP_c0 + Isopentadecanoyllipoteichoic_acid_n=24__linked__N-acetyl-D-glucosamine_c0 </t>
+  </si>
+  <si>
+    <t>rxn10314_c0</t>
+  </si>
+  <si>
+    <t>anteisopentadecanoyl-lipoteichoic acid synthesis n=24 linked N-acetylglucosamine substituted c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 UDP-N-acetylglucosamine_c0 + Anteisopentadecanoyllipoteichoic_acid_n=24__linked__unsubstituted_c0  &lt;=&gt; 24 UDP_c0 + Anteisopentadecanoyllipoteichoic_acid_n=24__linked__N-acetyl-D-glucosamine_c0 </t>
+  </si>
+  <si>
+    <t>rxn10315_c0</t>
+  </si>
+  <si>
+    <t>isohexadecanoyl-lipoteichoic acid synthesis n=24 linked N-acetylglucosamine substituted c0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 UDP-N-acetylglucosamine_c0 + Isohexadecanoyllipoteichoic_acid_n=24__linked__unsubstituted_c0  &lt;=&gt; 24 UDP_c0 + Isohexadecanoyllipoteichoic_acid_n=24__linked__N-acetyl-D-glucosamine_c0 </t>
+  </si>
+  <si>
+    <t>Reaction ID</t>
+  </si>
+  <si>
+    <t>Reaction Name</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -349,12 +675,414 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="254.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>